<commit_message>
last update: * change the gender code to M= 0 and F = 1 * column names corrected
</commit_message>
<xml_diff>
--- a/CleanData/Evaluation Data OMSU.xlsx
+++ b/CleanData/Evaluation Data OMSU.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="15460" tabRatio="745"/>
+    <workbookView xWindow="-38480" yWindow="900" windowWidth="20500" windowHeight="15460" tabRatio="745" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PreQOld" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="PostQModern" sheetId="5" r:id="rId5"/>
     <sheet name="Pre-Post-Test-Modernized" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,27 +36,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="121">
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Unuversity Year</t>
-  </si>
-  <si>
-    <t>Faculty</t>
-  </si>
-  <si>
-    <t>Average School  Math.</t>
-  </si>
-  <si>
-    <t>Average Univer. Math.</t>
-  </si>
-  <si>
-    <t>Compare with classmates</t>
-  </si>
   <si>
     <t>N1</t>
   </si>
@@ -399,6 +378,27 @@
   <si>
     <t>ICS16Stud22</t>
   </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>university year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faculty    </t>
+  </si>
+  <si>
+    <t>asm</t>
+  </si>
+  <si>
+    <t>aum</t>
+  </si>
+  <si>
+    <t>cwc</t>
+  </si>
 </sst>
 </file>
 
@@ -484,13 +484,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,114 +774,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:42" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="AI1" s="4"/>
       <c r="AJ1" s="4"/>
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -996,7 +996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -1100,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1204,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1308,7 +1308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1412,7 +1412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1516,7 +1516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -1620,7 +1620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -1724,7 +1724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -1828,7 +1828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -1932,7 +1932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -2036,7 +2036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>4.5</v>
@@ -2140,7 +2140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -2244,7 +2244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -2348,7 +2348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -2452,7 +2452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -2556,7 +2556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -2660,7 +2660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E19">
         <v>5</v>
@@ -2774,8 +2774,8 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>38</v>
+      <c r="D20" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E20">
         <v>5</v>
@@ -2868,7 +2868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2878,8 +2878,8 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>38</v>
+      <c r="D21" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -2972,7 +2972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2982,8 +2982,8 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>38</v>
+      <c r="D22" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -3076,7 +3076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3086,8 +3086,8 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>38</v>
+      <c r="D23" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -3180,7 +3180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3190,8 +3190,8 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>38</v>
+      <c r="D24" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -3284,7 +3284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -3294,8 +3294,8 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>38</v>
+      <c r="D25" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -3385,7 +3385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3395,8 +3395,8 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>38</v>
+      <c r="D26" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E26">
         <v>5</v>
@@ -3489,7 +3489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -3499,8 +3499,8 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>38</v>
+      <c r="D27" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E27">
         <v>5</v>
@@ -3593,7 +3593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3603,8 +3603,8 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>38</v>
+      <c r="D28" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -3697,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3707,8 +3707,8 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>38</v>
+      <c r="D29" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -3801,7 +3801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -3811,8 +3811,8 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>38</v>
+      <c r="D30" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -3905,7 +3905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -3915,8 +3915,8 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>38</v>
+      <c r="D31" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -4009,7 +4009,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0</v>
       </c>
@@ -4019,8 +4019,8 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>38</v>
+      <c r="D32" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E32">
         <v>5</v>
@@ -4113,7 +4113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -4123,8 +4123,8 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>38</v>
+      <c r="D33" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -4217,7 +4217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -4227,8 +4227,8 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>38</v>
+      <c r="D34" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -4321,7 +4321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0</v>
       </c>
@@ -4331,8 +4331,8 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>38</v>
+      <c r="D35" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -4425,7 +4425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -4435,8 +4435,8 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>38</v>
+      <c r="D36" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -4529,7 +4529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -4539,8 +4539,8 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>38</v>
+      <c r="D37" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -4633,7 +4633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0</v>
       </c>
@@ -4643,8 +4643,8 @@
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>38</v>
+      <c r="D38" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -4737,7 +4737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -4747,8 +4747,8 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>38</v>
+      <c r="D39" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E39">
         <v>5</v>
@@ -4852,113 +4852,113 @@
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D17"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:37" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
@@ -4975,7 +4975,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -5068,7 +5068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -5172,7 +5172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -5276,7 +5276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -5380,7 +5380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -5484,7 +5484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -5588,7 +5588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -5692,7 +5692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -5703,7 +5703,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -5796,7 +5796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -5900,7 +5900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -6004,7 +6004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -6108,7 +6108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -6212,7 +6212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -6223,7 +6223,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>5</v>
@@ -6316,7 +6316,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -6420,7 +6420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>4.5</v>
@@ -6524,7 +6524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -6638,8 +6638,8 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>38</v>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -6732,7 +6732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0</v>
       </c>
@@ -6742,8 +6742,8 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>38</v>
+      <c r="D19" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -6836,7 +6836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -6846,8 +6846,8 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>38</v>
+      <c r="D20" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -6940,7 +6940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -6950,8 +6950,8 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>38</v>
+      <c r="D21" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -7044,7 +7044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -7054,8 +7054,8 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>38</v>
+      <c r="D22" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -7148,7 +7148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -7158,8 +7158,8 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>38</v>
+      <c r="D23" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E23">
         <v>5</v>
@@ -7252,7 +7252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0</v>
       </c>
@@ -7262,8 +7262,8 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>38</v>
+      <c r="D24" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -7356,7 +7356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0</v>
       </c>
@@ -7366,8 +7366,8 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>38</v>
+      <c r="D25" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -7460,7 +7460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0</v>
       </c>
@@ -7470,8 +7470,8 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>38</v>
+      <c r="D26" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -7564,7 +7564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -7574,8 +7574,8 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>38</v>
+      <c r="D27" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -7668,7 +7668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -7678,8 +7678,8 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>38</v>
+      <c r="D28" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -7772,7 +7772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -7782,8 +7782,8 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>38</v>
+      <c r="D29" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -7876,7 +7876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -7886,8 +7886,8 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>38</v>
+      <c r="D30" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -7980,7 +7980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -7990,8 +7990,8 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>38</v>
+      <c r="D31" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -8084,7 +8084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -8094,8 +8094,8 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>38</v>
+      <c r="D32" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -8188,7 +8188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -8198,8 +8198,8 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>38</v>
+      <c r="D33" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -8292,7 +8292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -8302,8 +8302,8 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>38</v>
+      <c r="D34" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -8396,7 +8396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -8406,8 +8406,8 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>38</v>
+      <c r="D35" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -8521,18 +8521,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>13</v>
@@ -8543,7 +8543,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>28</v>
@@ -8554,7 +8554,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -8565,7 +8565,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>38</v>
@@ -8576,7 +8576,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>41</v>
@@ -8587,7 +8587,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>19</v>
@@ -8598,7 +8598,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>25</v>
@@ -8609,7 +8609,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8620,7 +8620,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B10">
         <v>31</v>
@@ -8631,7 +8631,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B11">
         <v>38</v>
@@ -8642,7 +8642,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -8653,7 +8653,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>16</v>
@@ -8664,7 +8664,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>28</v>
@@ -8675,7 +8675,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>25</v>
@@ -8686,7 +8686,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>28</v>
@@ -8697,7 +8697,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B17">
         <v>22</v>
@@ -8708,7 +8708,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B18">
         <v>44</v>
@@ -8719,7 +8719,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>34</v>
@@ -8730,7 +8730,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B20">
         <v>22</v>
@@ -8741,7 +8741,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B21">
         <v>19</v>
@@ -8752,7 +8752,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B22">
         <v>25</v>
@@ -8763,7 +8763,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B23">
         <v>28</v>
@@ -8774,7 +8774,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B24">
         <v>41</v>
@@ -8785,7 +8785,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B25">
         <v>28</v>
@@ -8796,7 +8796,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B26">
         <v>16</v>
@@ -8807,7 +8807,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B27">
         <v>19</v>
@@ -8818,7 +8818,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B28">
         <v>31</v>
@@ -8829,7 +8829,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B29">
         <v>44</v>
@@ -8840,7 +8840,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B30">
         <v>19</v>
@@ -8851,7 +8851,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -8862,7 +8862,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B32">
         <v>16</v>
@@ -8873,7 +8873,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B33">
         <v>38</v>
@@ -8884,7 +8884,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B34">
         <v>13</v>
@@ -8895,7 +8895,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B35">
         <v>16</v>
@@ -8906,7 +8906,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B36">
         <v>22</v>
@@ -8917,7 +8917,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B37">
         <v>25</v>
@@ -8928,7 +8928,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B38">
         <v>41</v>
@@ -8951,114 +8951,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP51"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:42" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="AI1" s="4"/>
       <c r="AJ1" s="4"/>
@@ -9080,7 +9080,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -9173,7 +9173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -9277,7 +9277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -9288,7 +9288,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -9381,7 +9381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -9485,7 +9485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -9496,7 +9496,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -9589,7 +9589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -9693,7 +9693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -9704,7 +9704,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -9797,7 +9797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -9901,7 +9901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -9912,7 +9912,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -10005,7 +10005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -10016,7 +10016,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -10109,7 +10109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -10213,7 +10213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>4.5</v>
@@ -10317,7 +10317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -10421,7 +10421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0</v>
       </c>
@@ -10432,7 +10432,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -10525,7 +10525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:42" ht="124" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -10536,7 +10536,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -10629,7 +10629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
@@ -10640,7 +10640,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -10733,7 +10733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -10744,7 +10744,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -10837,7 +10837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -10848,7 +10848,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -10941,7 +10941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -10952,7 +10952,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>5</v>
@@ -11045,7 +11045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -11056,7 +11056,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -11149,7 +11149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0</v>
       </c>
@@ -11160,7 +11160,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -11253,7 +11253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -11357,7 +11357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -11368,7 +11368,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -11461,7 +11461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -11472,7 +11472,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -11565,7 +11565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0</v>
       </c>
@@ -11576,7 +11576,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -11679,8 +11679,8 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>38</v>
+      <c r="D27" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E27">
         <v>5</v>
@@ -11773,7 +11773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -11783,8 +11783,8 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>38</v>
+      <c r="D28" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -11877,7 +11877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -11887,8 +11887,8 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>38</v>
+      <c r="D29" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -11981,7 +11981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -11991,8 +11991,8 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>38</v>
+      <c r="D30" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -12085,7 +12085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0</v>
       </c>
@@ -12095,8 +12095,8 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>38</v>
+      <c r="D31" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -12189,7 +12189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -12199,8 +12199,8 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>38</v>
+      <c r="D32" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -12293,7 +12293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -12303,8 +12303,8 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>38</v>
+      <c r="D33" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -12397,7 +12397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -12407,8 +12407,8 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>38</v>
+      <c r="D34" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -12501,7 +12501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -12511,8 +12511,8 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>38</v>
+      <c r="D35" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -12605,7 +12605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -12615,8 +12615,8 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>38</v>
+      <c r="D36" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -12709,7 +12709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -12719,8 +12719,8 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>38</v>
+      <c r="D37" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -12813,7 +12813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -12823,8 +12823,8 @@
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>38</v>
+      <c r="D38" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E38">
         <v>5</v>
@@ -12917,7 +12917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -12927,8 +12927,8 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>38</v>
+      <c r="D39" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E39">
         <v>5</v>
@@ -13021,7 +13021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -13031,8 +13031,8 @@
       <c r="C40">
         <v>1</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>38</v>
+      <c r="D40" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -13125,7 +13125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -13135,8 +13135,8 @@
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>38</v>
+      <c r="D41" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -13229,7 +13229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -13239,8 +13239,8 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>38</v>
+      <c r="D42" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -13333,7 +13333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -13343,8 +13343,8 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>38</v>
+      <c r="D43" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -13437,7 +13437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0</v>
       </c>
@@ -13447,8 +13447,8 @@
       <c r="C44">
         <v>1</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>38</v>
+      <c r="D44" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E44">
         <v>5</v>
@@ -13541,7 +13541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0</v>
       </c>
@@ -13551,8 +13551,8 @@
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>38</v>
+      <c r="D45" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E45">
         <v>5</v>
@@ -13645,7 +13645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -13655,8 +13655,8 @@
       <c r="C46">
         <v>1</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>38</v>
+      <c r="D46" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -13749,7 +13749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -13759,8 +13759,8 @@
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>38</v>
+      <c r="D47" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E47">
         <v>4</v>
@@ -13853,7 +13853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
@@ -13863,8 +13863,8 @@
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>38</v>
+      <c r="D48" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E48">
         <v>4</v>
@@ -13957,7 +13957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -13967,8 +13967,8 @@
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>38</v>
+      <c r="D49" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -14061,7 +14061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>0</v>
       </c>
@@ -14071,8 +14071,8 @@
       <c r="C50">
         <v>1</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>38</v>
+      <c r="D50" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E50">
         <v>4</v>
@@ -14165,7 +14165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:34" ht="190" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -14175,8 +14175,8 @@
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>38</v>
+      <c r="D51" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -14279,114 +14279,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D45"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:37" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
@@ -14403,7 +14403,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -14496,7 +14496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -14507,7 +14507,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -14600,7 +14600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -14611,7 +14611,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>4.5</v>
@@ -14704,7 +14704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -14715,7 +14715,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -14808,7 +14808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -14819,7 +14819,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -14912,7 +14912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -14923,7 +14923,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -15016,7 +15016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -15027,7 +15027,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -15120,7 +15120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -15131,7 +15131,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -15224,7 +15224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -15235,7 +15235,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -15328,7 +15328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -15339,7 +15339,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -15432,7 +15432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -15443,7 +15443,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -15536,7 +15536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -15547,7 +15547,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -15640,7 +15640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -15651,7 +15651,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -15744,7 +15744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -15755,7 +15755,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -15848,7 +15848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="124" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -15859,7 +15859,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -15952,7 +15952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -15963,7 +15963,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -16056,7 +16056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -16067,7 +16067,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -16160,7 +16160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -16171,7 +16171,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E19">
         <v>4.5</v>
@@ -16264,7 +16264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0</v>
       </c>
@@ -16275,7 +16275,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>5</v>
@@ -16368,7 +16368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -16379,7 +16379,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -16472,7 +16472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0</v>
       </c>
@@ -16483,7 +16483,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -16576,7 +16576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -16587,7 +16587,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -16680,7 +16680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -16691,7 +16691,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -16784,7 +16784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="124" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0</v>
       </c>
@@ -16795,7 +16795,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -16898,8 +16898,8 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>38</v>
+      <c r="D26" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E26">
         <v>5</v>
@@ -16992,7 +16992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -17002,8 +17002,8 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>38</v>
+      <c r="D27" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -17096,7 +17096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -17106,8 +17106,8 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>38</v>
+      <c r="D28" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -17200,7 +17200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -17210,8 +17210,8 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>38</v>
+      <c r="D29" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -17304,7 +17304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0</v>
       </c>
@@ -17314,8 +17314,8 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>38</v>
+      <c r="D30" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E30">
         <v>4</v>
@@ -17408,7 +17408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -17418,8 +17418,8 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>38</v>
+      <c r="D31" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -17512,7 +17512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -17522,8 +17522,8 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>38</v>
+      <c r="D32" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -17616,7 +17616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0</v>
       </c>
@@ -17626,8 +17626,8 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>38</v>
+      <c r="D33" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -17720,7 +17720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -17730,8 +17730,8 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>38</v>
+      <c r="D34" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -17824,7 +17824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -17834,8 +17834,8 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>38</v>
+      <c r="D35" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -17928,7 +17928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0</v>
       </c>
@@ -17938,8 +17938,8 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>38</v>
+      <c r="D36" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E36">
         <v>5</v>
@@ -18032,7 +18032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -18042,8 +18042,8 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>38</v>
+      <c r="D37" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E37">
         <v>5</v>
@@ -18136,7 +18136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -18146,8 +18146,8 @@
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>38</v>
+      <c r="D38" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -18240,7 +18240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -18250,8 +18250,8 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>38</v>
+      <c r="D39" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E39">
         <v>5</v>
@@ -18344,7 +18344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -18354,8 +18354,8 @@
       <c r="C40">
         <v>1</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>38</v>
+      <c r="D40" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -18448,7 +18448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
@@ -18458,8 +18458,8 @@
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>38</v>
+      <c r="D41" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E41">
         <v>5</v>
@@ -18552,7 +18552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -18562,8 +18562,8 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>38</v>
+      <c r="D42" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -18653,7 +18653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -18663,8 +18663,8 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>38</v>
+      <c r="D43" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -18757,7 +18757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0</v>
       </c>
@@ -18767,8 +18767,8 @@
       <c r="C44">
         <v>1</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>38</v>
+      <c r="D44" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E44">
         <v>4</v>
@@ -18861,7 +18861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="175" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -18871,8 +18871,8 @@
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>38</v>
+      <c r="D45" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -18986,18 +18986,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B2">
         <v>22</v>
@@ -19008,7 +19008,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>28</v>
@@ -19019,7 +19019,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>59</v>
@@ -19030,7 +19030,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <v>13</v>
@@ -19041,7 +19041,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <v>41</v>
@@ -19052,7 +19052,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>41</v>
@@ -19063,7 +19063,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>41</v>
@@ -19074,7 +19074,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B9">
         <v>44</v>
@@ -19085,7 +19085,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B10">
         <v>19</v>
@@ -19096,7 +19096,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>28</v>
@@ -19107,7 +19107,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>25</v>
@@ -19118,7 +19118,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B13">
         <v>28</v>
@@ -19129,7 +19129,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B14">
         <v>31</v>
@@ -19140,7 +19140,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B15">
         <v>22</v>
@@ -19151,7 +19151,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B16">
         <v>28</v>
@@ -19162,7 +19162,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B17">
         <v>22</v>
@@ -19173,7 +19173,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B18">
         <v>34</v>
@@ -19184,7 +19184,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B19">
         <v>13</v>
@@ -19195,7 +19195,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B20">
         <v>38</v>
@@ -19206,7 +19206,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B21">
         <v>31</v>
@@ -19217,7 +19217,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B22">
         <v>53</v>
@@ -19228,7 +19228,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B23">
         <v>34</v>
@@ -19239,7 +19239,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B24">
         <v>31</v>
@@ -19250,7 +19250,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B25">
         <v>22</v>
@@ -19261,7 +19261,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B26">
         <v>31</v>
@@ -19272,7 +19272,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B27">
         <v>22</v>
@@ -19283,7 +19283,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B28">
         <v>34</v>
@@ -19294,7 +19294,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -19305,7 +19305,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B30">
         <v>28</v>
@@ -19316,7 +19316,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B31">
         <v>19</v>
@@ -19327,7 +19327,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B32">
         <v>28</v>
@@ -19338,7 +19338,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B33">
         <v>31</v>
@@ -19349,7 +19349,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B34">
         <v>28</v>
@@ -19360,7 +19360,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B35">
         <v>22</v>
@@ -19371,7 +19371,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B36">
         <v>31</v>
@@ -19382,7 +19382,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B37">
         <v>38</v>
@@ -19393,7 +19393,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B38">
         <v>47</v>
@@ -19404,7 +19404,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B39">
         <v>22</v>
@@ -19415,7 +19415,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B40">
         <v>19</v>
@@ -19426,7 +19426,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B41">
         <v>22</v>
@@ -19437,7 +19437,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B42">
         <v>31</v>
@@ -19448,7 +19448,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B43">
         <v>41</v>
@@ -19459,7 +19459,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B44">
         <v>34</v>
@@ -19470,7 +19470,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B45">
         <v>53</v>
@@ -19481,7 +19481,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B46">
         <v>34</v>

</xml_diff>